<commit_message>
Agrega pdf's y arregla nombres
</commit_message>
<xml_diff>
--- a/slides/data/template.xlsx
+++ b/slides/data/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgpen\Documents\R4Finance\slides\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4800184C-11B9-44E7-AFC1-C6E6A075868A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1307C7-2B9B-412B-BB7F-622EAD52594E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -775,10 +775,10 @@
     <t>q_us</t>
   </si>
   <si>
-    <t>concept</t>
+    <t>Pretax IncomeBAL</t>
   </si>
   <si>
-    <t>Pretax IncomeBAL</t>
+    <t>concept</t>
   </si>
 </sst>
 </file>
@@ -23302,7 +23302,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23315,7 +23315,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -23568,7 +23568,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B12" s="8">
         <v>2597.7020000000002</v>

</xml_diff>

<commit_message>
Corrige formato de los nombres y agrega set de slides 5
</commit_message>
<xml_diff>
--- a/slides/data/template.xlsx
+++ b/slides/data/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgpen\Documents\R4Finance\slides\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1307C7-2B9B-412B-BB7F-622EAD52594E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A7B5A6-ADD5-49B7-BB4A-6F75B72F5394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regressors" sheetId="4" r:id="rId1"/>
@@ -23301,7 +23301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -23746,7 +23746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F34427-1E59-4C8C-A12C-3CCE4BEA0C01}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -23760,7 +23760,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>240</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>2</v>

</xml_diff>